<commit_message>
superdataset-24 (hybrid model, mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-12.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-12.xlsx
@@ -10,6 +10,10 @@
     <sheet name="pos vs negative" sheetId="1" r:id="rId1"/>
     <sheet name="hybrid-3" sheetId="3" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'hybrid-3'!$T$4:$T$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'hybrid-3'!$U$4:$U$20</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -793,7 +797,7 @@
     <c:plotArea>
       <c:layout/>
       <c:barChart>
-        <c:barDir val="bar"/>
+        <c:barDir val="col"/>
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
@@ -955,7 +959,6 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="227"/>
-        <c:overlap val="-48"/>
         <c:axId val="1421546911"/>
         <c:axId val="1421547327"/>
       </c:barChart>
@@ -965,7 +968,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1016,7 +1019,7 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4128,8 +4131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R15" sqref="R15"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC28" sqref="AC28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>